<commit_message>
"Moervaart Depresie ready,  mf6lab now has its final structure.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/MoervaarDpr/MoervaarDpr.xlsx
+++ b/Projects/VoortoetsAGT/cases/MoervaarDpr/MoervaarDpr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/VoortoetsAGT/cases/MoervaarDpr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/MoervaarDpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF577403-47A7-BC47-A828-353EAC24BF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDDA38A-F3DB-7440-83F7-69CE1A1615E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="-25980" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="-18660" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="420">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1438,6 +1438,33 @@
   </si>
   <si>
     <t>Ss</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>lightskyblue</t>
+  </si>
+  <si>
+    <t>lightsalmon</t>
+  </si>
+  <si>
+    <t>violet</t>
+  </si>
+  <si>
+    <t>chocolate</t>
+  </si>
+  <si>
+    <t>yellowgreen</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1595,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1589,6 +1616,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -12560,15 +12588,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+    <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -12588,13 +12619,16 @@
         <v>410</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12613,14 +12647,17 @@
       <c r="F2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12639,14 +12676,17 @@
       <c r="F3" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12665,14 +12705,17 @@
       <c r="F4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12691,14 +12734,17 @@
       <c r="F5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12717,14 +12763,17 @@
       <c r="F6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12743,14 +12792,17 @@
       <c r="F7" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12769,14 +12821,17 @@
       <c r="F8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12795,242 +12850,291 @@
       <c r="F9" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>